<commit_message>
uploading patient data file
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PC001.xlsx
+++ b/client/src/data/patients/PC001.xlsx
@@ -34,15 +34,12 @@
     <t>Observation 6</t>
   </si>
   <si>
-    <t>Centre de Recherche et des Essais Cliniques                                   21 Rue Du Jeudi Matin                                                             22076 Mouton de Van                                                               Projet: P-2021A22L                                                               Investigateur: I-7031B                                                      Promoteur: P-8922A</t>
+    <t>Centre de Recherche et des Essais Cliniques                                   21 Rue Du Jeudi Matin                                                             22076 Mouton de Van                                                               Projet: P94C001FR                                                               Investigateur: I-7031B                                                      Promoteur: P-8922A</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2001-09-08T08:40:00</t>
-  </si>
-  <si>
     <t>Poids</t>
   </si>
   <si>
@@ -52,10 +49,13 @@
     <t>Effets secondaires</t>
   </si>
   <si>
-    <t>non</t>
+    <t>0.2</t>
   </si>
   <si>
     <t>Effets secondaires graves</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>Age</t>
@@ -89,8 +89,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -278,7 +279,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -314,6 +315,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -1499,149 +1503,149 @@
       <c r="C3" t="s" s="11">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="12">
-        <v>9</v>
+      <c r="D3" s="12">
+        <v>44326.615185185183</v>
       </c>
       <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" ht="22.2" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" t="s" s="14">
-        <v>10</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" t="s" s="15">
+        <v>9</v>
+      </c>
+      <c r="D4" s="16">
         <v>30</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" ht="22.2" customHeight="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" t="s" s="18">
-        <v>11</v>
-      </c>
-      <c r="D5" s="19">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" t="s" s="19">
+        <v>10</v>
+      </c>
+      <c r="D5" s="20">
         <v>1.4</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" ht="22.2" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" t="s" s="14">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" t="s" s="15">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s" s="22">
         <v>12</v>
       </c>
-      <c r="D6" t="s" s="21">
-        <v>13</v>
-      </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" ht="22.2" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" t="s" s="18">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s" s="23">
         <v>14</v>
       </c>
-      <c r="D7" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" ht="22.2" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" t="s" s="14">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" t="s" s="15">
         <v>15</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="24">
         <v>27</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" ht="22.2" customHeight="1">
-      <c r="A9" t="s" s="24">
+      <c r="A9" t="s" s="25">
         <v>16</v>
       </c>
-      <c r="B9" t="s" s="14">
+      <c r="B9" t="s" s="15">
         <v>17</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" ht="22.2" customHeight="1">
-      <c r="A10" t="s" s="24">
+      <c r="A10" t="s" s="25">
         <v>18</v>
       </c>
-      <c r="B10" t="s" s="18">
+      <c r="B10" t="s" s="19">
         <v>19</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" ht="22.2" customHeight="1">
-      <c r="A11" t="s" s="24">
+      <c r="A11" t="s" s="25">
         <v>20</v>
       </c>
-      <c r="B11" t="s" s="14">
+      <c r="B11" t="s" s="15">
         <v>21</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" ht="22.2" customHeight="1">
-      <c r="A12" t="s" s="24">
+      <c r="A12" t="s" s="25">
         <v>22</v>
       </c>
-      <c r="B12" t="s" s="18">
+      <c r="B12" t="s" s="19">
         <v>23</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
some changes patient data page
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PC001.xlsx
+++ b/client/src/data/patients/PC001.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>Données Patient</t>
   </si>
@@ -49,16 +49,13 @@
     <t>Effets secondaires</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
     <t>Effets secondaires graves</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>Observation</t>
   </si>
   <si>
     <t>ID</t>
@@ -89,9 +86,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="yyyy-mm-dd hh:mm:ss"/>
+    <numFmt numFmtId="60" formatCode="0.0"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -279,7 +277,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -346,17 +344,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1443,7 +1450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1548,35 +1555,35 @@
       <c r="C6" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="22">
-        <v>12</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+      <c r="D6" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" ht="22.2" customHeight="1">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s" s="23">
-        <v>14</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
+        <v>12</v>
+      </c>
+      <c r="D7" s="25">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" ht="22.2" customHeight="1">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" t="s" s="15">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="24">
         <v>27</v>
@@ -1588,26 +1595,26 @@
       <c r="I8" s="17"/>
     </row>
     <row r="9" ht="22.2" customHeight="1">
-      <c r="A9" t="s" s="25">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s" s="15">
-        <v>17</v>
+      <c r="A9" t="s" s="27">
+        <v>14</v>
+      </c>
+      <c r="B9" s="28">
+        <v>1</v>
       </c>
       <c r="C9" s="18"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" ht="22.2" customHeight="1">
-      <c r="A10" t="s" s="25">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s" s="19">
-        <v>19</v>
+      <c r="A10" t="s" s="27">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s" s="15">
+        <v>16</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -1618,26 +1625,26 @@
       <c r="I10" s="18"/>
     </row>
     <row r="11" ht="22.2" customHeight="1">
-      <c r="A11" t="s" s="25">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s" s="15">
-        <v>21</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="A11" t="s" s="27">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" ht="22.2" customHeight="1">
-      <c r="A12" t="s" s="25">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s" s="19">
-        <v>23</v>
+      <c r="A12" t="s" s="27">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s" s="15">
+        <v>20</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -1647,12 +1654,27 @@
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
+    <row r="13" ht="22.2" customHeight="1">
+      <c r="A13" t="s" s="27">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s" s="19">
+        <v>22</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:B8"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="C9:I12"/>
+    <mergeCell ref="C9:I13"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
storing patient data to ipfs and cid to ethereum
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PC001.xlsx
+++ b/client/src/data/patients/PC001.xlsx
@@ -277,7 +277,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -329,31 +329,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1508,7 +1511,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="12">
-        <v>44326.615185185183</v>
+        <v>44327.930995370371</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="13"/>
@@ -1525,21 +1528,11 @@
       <c r="D4" s="16">
         <v>30</v>
       </c>
-      <c r="E4" s="17">
-        <v>1</v>
-      </c>
-      <c r="F4" s="17">
-        <v>1</v>
-      </c>
-      <c r="G4" s="17">
-        <v>1</v>
-      </c>
-      <c r="H4" s="17">
-        <v>1</v>
-      </c>
-      <c r="I4" s="17">
-        <v>1</v>
-      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" ht="22.2" customHeight="1">
       <c r="A5" s="18"/>
@@ -1550,21 +1543,11 @@
       <c r="D5" s="20">
         <v>1.4</v>
       </c>
-      <c r="E5" s="21">
-        <v>1</v>
-      </c>
-      <c r="F5" s="21">
-        <v>1</v>
-      </c>
-      <c r="G5" s="21">
-        <v>1</v>
-      </c>
-      <c r="H5" s="21">
-        <v>1</v>
-      </c>
-      <c r="I5" s="21">
-        <v>1</v>
-      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" ht="22.2" customHeight="1">
       <c r="A6" s="14"/>
@@ -1575,21 +1558,11 @@
       <c r="D6" s="22">
         <v>0.2</v>
       </c>
-      <c r="E6" s="23">
-        <v>1</v>
-      </c>
-      <c r="F6" s="17">
-        <v>1</v>
-      </c>
-      <c r="G6" s="17">
-        <v>1</v>
-      </c>
-      <c r="H6" s="17">
-        <v>1</v>
-      </c>
-      <c r="I6" s="17">
-        <v>1</v>
-      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
     </row>
     <row r="7" ht="22.2" customHeight="1">
       <c r="A7" s="18"/>
@@ -1597,24 +1570,14 @@
       <c r="C7" t="s" s="19">
         <v>12</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="25">
         <v>0</v>
       </c>
-      <c r="E7" s="24">
-        <v>1</v>
-      </c>
-      <c r="F7" s="21">
-        <v>1</v>
-      </c>
-      <c r="G7" s="21">
-        <v>1</v>
-      </c>
-      <c r="H7" s="21">
-        <v>1</v>
-      </c>
-      <c r="I7" s="21">
-        <v>1</v>
-      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" ht="22.2" customHeight="1">
       <c r="A8" s="14"/>
@@ -1622,21 +1585,21 @@
       <c r="C8" t="s" s="15">
         <v>13</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="24">
         <v>27</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" ht="22.2" customHeight="1">
-      <c r="A9" t="s" s="26">
+      <c r="A9" t="s" s="27">
         <v>14</v>
       </c>
-      <c r="B9" s="27">
-        <v>6</v>
+      <c r="B9" s="28">
+        <v>1</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -1647,7 +1610,7 @@
       <c r="I9" s="18"/>
     </row>
     <row r="10" ht="22.2" customHeight="1">
-      <c r="A10" t="s" s="26">
+      <c r="A10" t="s" s="27">
         <v>15</v>
       </c>
       <c r="B10" t="s" s="15">
@@ -1662,7 +1625,7 @@
       <c r="I10" s="18"/>
     </row>
     <row r="11" ht="22.2" customHeight="1">
-      <c r="A11" t="s" s="26">
+      <c r="A11" t="s" s="27">
         <v>17</v>
       </c>
       <c r="B11" t="s" s="19">
@@ -1677,7 +1640,7 @@
       <c r="I11" s="18"/>
     </row>
     <row r="12" ht="22.2" customHeight="1">
-      <c r="A12" t="s" s="26">
+      <c r="A12" t="s" s="27">
         <v>19</v>
       </c>
       <c r="B12" t="s" s="15">
@@ -1692,7 +1655,7 @@
       <c r="I12" s="18"/>
     </row>
     <row r="13" ht="22.2" customHeight="1">
-      <c r="A13" t="s" s="26">
+      <c r="A13" t="s" s="27">
         <v>21</v>
       </c>
       <c r="B13" t="s" s="19">

</xml_diff>

<commit_message>
patient data page changes
</commit_message>
<xml_diff>
--- a/client/src/data/patients/PC001.xlsx
+++ b/client/src/data/patients/PC001.xlsx
@@ -329,6 +329,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -341,6 +344,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -350,13 +356,7 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1513,9 +1513,15 @@
       <c r="D3" s="12">
         <v>44327.930995370371</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="E3" s="12">
+        <v>44328.160069444442</v>
+      </c>
+      <c r="F3" s="12">
+        <v>44328.177731481483</v>
+      </c>
+      <c r="G3" s="12">
+        <v>44328.186539351853</v>
+      </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
@@ -1528,26 +1534,38 @@
       <c r="D4" s="16">
         <v>30</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="E4" s="17">
+        <v>30</v>
+      </c>
+      <c r="F4" s="17">
+        <v>31</v>
+      </c>
+      <c r="G4" s="17">
+        <v>30</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" ht="22.2" customHeight="1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" t="s" s="19">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" t="s" s="20">
         <v>10</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="21">
         <v>1.4</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="E5" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="22">
+        <v>1.3</v>
+      </c>
+      <c r="G5" s="22">
+        <v>1.2</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" ht="22.2" customHeight="1">
       <c r="A6" s="14"/>
@@ -1555,29 +1573,41 @@
       <c r="C6" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="24">
         <v>0.2</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
+      <c r="E6" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" ht="22.2" customHeight="1">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" t="s" s="19">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" t="s" s="20">
         <v>12</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="26">
         <v>0</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
+      <c r="E7" s="26">
+        <v>0</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0</v>
+      </c>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" ht="22.2" customHeight="1">
       <c r="A8" s="14"/>
@@ -1585,29 +1615,35 @@
       <c r="C8" t="s" s="15">
         <v>13</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="17">
         <v>27</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="E8" s="17">
+        <v>27</v>
+      </c>
+      <c r="F8" s="17">
+        <v>27</v>
+      </c>
+      <c r="G8" s="17">
+        <v>27</v>
+      </c>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" ht="22.2" customHeight="1">
       <c r="A9" t="s" s="27">
         <v>14</v>
       </c>
       <c r="B9" s="28">
-        <v>1</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" ht="22.2" customHeight="1">
       <c r="A10" t="s" s="27">
@@ -1616,28 +1652,28 @@
       <c r="B10" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" ht="22.2" customHeight="1">
       <c r="A11" t="s" s="27">
         <v>17</v>
       </c>
-      <c r="B11" t="s" s="19">
+      <c r="B11" t="s" s="20">
         <v>18</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" ht="22.2" customHeight="1">
       <c r="A12" t="s" s="27">
@@ -1646,28 +1682,28 @@
       <c r="B12" t="s" s="15">
         <v>20</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" ht="22.2" customHeight="1">
       <c r="A13" t="s" s="27">
         <v>21</v>
       </c>
-      <c r="B13" t="s" s="19">
+      <c r="B13" t="s" s="20">
         <v>22</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>